<commit_message>
with pdf and excel
</commit_message>
<xml_diff>
--- a/Data/summary_statistics.xlsx
+++ b/Data/summary_statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\DataMohammed\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAE2F97-A9EE-4EF4-BF33-B395B1D3A73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45950712-F7DC-4E68-BD48-B29DBD44F2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>